<commit_message>
Dashboard has been updated to include new features
</commit_message>
<xml_diff>
--- a/source/source_CRPM_exceptions.xlsx
+++ b/source/source_CRPM_exceptions.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.wiepking\Projects\CRPM check\source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCF2C33-552F-4B21-8880-BAD0F8B56C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96CB0273-D9BB-42BC-87F3-DF2ED37F889F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25245" yWindow="2685" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="103">
   <si>
     <t>Rule_Type</t>
   </si>
@@ -264,6 +264,87 @@
   </si>
   <si>
     <t>GRPNT,NOTAX</t>
+  </si>
+  <si>
+    <t>COMPBKF,COMPBKF,COMPHU,COMP,COMP,COMP,COMP,COMB,COMB,COMB,COMB,COMB,COMB,COMB,COMB,COMB,COMB,COMPRAOK,COMPRABK,EMPCOMP,HCA7,HCB9,HCDX,HCB8,HCDW</t>
+  </si>
+  <si>
+    <t>ADT,MSB,NYB,NYT,BBB,BNS,CDT,LAD,MBR,MPK,MWC,SFU,SPS,SSL,WCA,WNM</t>
+  </si>
+  <si>
+    <t>COMP rates do not trigger tax calculations</t>
+  </si>
+  <si>
+    <t>NYB</t>
+  </si>
+  <si>
+    <t>NYT</t>
+  </si>
+  <si>
+    <t>AMA</t>
+  </si>
+  <si>
+    <t>AMS</t>
+  </si>
+  <si>
+    <t>AMZ</t>
+  </si>
+  <si>
+    <t>GEN</t>
+  </si>
+  <si>
+    <t>KLB</t>
+  </si>
+  <si>
+    <t>PCG</t>
+  </si>
+  <si>
+    <t>PGL</t>
+  </si>
+  <si>
+    <t>PLD</t>
+  </si>
+  <si>
+    <t>POP</t>
+  </si>
+  <si>
+    <t>RTM</t>
+  </si>
+  <si>
+    <t>ZUR</t>
+  </si>
+  <si>
+    <t>COMPBKF</t>
+  </si>
+  <si>
+    <t>COMPHU</t>
+  </si>
+  <si>
+    <t>MICRO</t>
+  </si>
+  <si>
+    <t>ECNRPKG</t>
+  </si>
+  <si>
+    <t>ECCOBK</t>
+  </si>
+  <si>
+    <t>HCA7</t>
+  </si>
+  <si>
+    <t>HCB9</t>
+  </si>
+  <si>
+    <t>HCDX</t>
+  </si>
+  <si>
+    <t>HCB8</t>
+  </si>
+  <si>
+    <t>COMPBKF,COMPHU,MICRO,ECNRPKG,HTNREF,ECCOBK,HCA7,HCB9,HCDX,HCB8</t>
+  </si>
+  <si>
+    <t>NYB,NYT,AMA,AMS,AMZ,GEN,KLB,PCG,PGL,PLD,POP,RIT,RTM,ZUR</t>
   </si>
 </sst>
 </file>
@@ -658,11 +739,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N137"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="180" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="180" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1568,7 +1649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="24" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>17</v>
       </c>
@@ -1667,26 +1748,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>30</v>
+        <v>17</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="1">
+        <v>108000</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="I31" s="7" t="s">
         <v>24</v>
@@ -1714,7 +1796,7 @@
         <v>12</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="H32" s="7" t="s">
         <v>30</v>
@@ -1731,16 +1813,14 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>43</v>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7" t="s">
@@ -1750,7 +1830,7 @@
         <v>39</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="I33" s="7" t="s">
         <v>24</v>
@@ -1763,10 +1843,69 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J34" s="2"/>
+      <c r="A34" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J34" s="9">
+        <v>45915</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="J35" s="2"/>
+      <c r="A35" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J35" s="9">
+        <v>45915</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J36" s="2"/>
@@ -1774,90 +1913,525 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="J37" s="2"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="str">
+        <f>_xlfn.TEXTJOIN(",",,B38:B51)</f>
+        <v>NYB,NYT,AMA,AMS,AMZ,GEN,KLB,PCG,PGL,PLD,POP,RIT,RTM,ZUR</v>
+      </c>
       <c r="J38" s="2"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
+        <v>93</v>
+      </c>
+      <c r="D39"/>
       <c r="J39" s="2"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40"/>
       <c r="J40" s="2"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" t="s">
+        <v>95</v>
+      </c>
+      <c r="D41"/>
       <c r="J41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42"/>
       <c r="J42" s="2"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" t="s">
+        <v>96</v>
+      </c>
+      <c r="D43"/>
       <c r="J43" s="2"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>85</v>
+      </c>
+      <c r="C44" t="s">
+        <v>97</v>
+      </c>
+      <c r="D44"/>
       <c r="J44" s="2"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C45" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45"/>
       <c r="J45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46"/>
       <c r="J46" s="2"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47"/>
       <c r="J47" s="2"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48"/>
+      <c r="D48"/>
       <c r="J48" s="2"/>
     </row>
-    <row r="49" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49"/>
+      <c r="D49"/>
       <c r="J49" s="2"/>
     </row>
-    <row r="50" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>90</v>
+      </c>
+      <c r="C50"/>
+      <c r="D50"/>
       <c r="J50" s="2"/>
     </row>
-    <row r="51" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51"/>
+      <c r="D51"/>
       <c r="J51" s="2"/>
     </row>
-    <row r="52" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
       <c r="J52" s="2"/>
     </row>
-    <row r="53" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
       <c r="J53" s="2"/>
     </row>
-    <row r="54" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
       <c r="J54" s="2"/>
     </row>
-    <row r="55" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
       <c r="J55" s="2"/>
     </row>
-    <row r="56" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
       <c r="J56" s="2"/>
     </row>
-    <row r="57" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
       <c r="J57" s="2"/>
     </row>
-    <row r="58" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B58"/>
+      <c r="C58"/>
+      <c r="D58"/>
       <c r="J58" s="2"/>
     </row>
-    <row r="59" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B59"/>
+      <c r="C59"/>
+      <c r="D59"/>
       <c r="J59" s="2"/>
     </row>
-    <row r="60" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
       <c r="J60" s="2"/>
     </row>
-    <row r="61" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
       <c r="J61" s="2"/>
     </row>
-    <row r="62" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B62"/>
+      <c r="C62"/>
+      <c r="D62"/>
       <c r="J62" s="2"/>
     </row>
-    <row r="63" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B63"/>
+      <c r="C63"/>
+      <c r="D63"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="64" spans="10:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B64"/>
+      <c r="C64"/>
+      <c r="D64"/>
       <c r="J64" s="2"/>
     </row>
+    <row r="65" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B65"/>
+      <c r="C65"/>
+      <c r="D65"/>
+    </row>
+    <row r="66" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B66"/>
+      <c r="C66"/>
+      <c r="D66"/>
+    </row>
+    <row r="67" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B67"/>
+      <c r="C67"/>
+      <c r="D67"/>
+    </row>
+    <row r="68" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B68"/>
+      <c r="C68"/>
+      <c r="D68"/>
+    </row>
+    <row r="69" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B69"/>
+      <c r="C69"/>
+      <c r="D69"/>
+    </row>
+    <row r="70" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B70"/>
+      <c r="C70"/>
+      <c r="D70"/>
+    </row>
+    <row r="71" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B71"/>
+      <c r="C71"/>
+      <c r="D71"/>
+    </row>
+    <row r="72" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B72"/>
+      <c r="C72"/>
+      <c r="D72"/>
+    </row>
+    <row r="73" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B73"/>
+      <c r="C73"/>
+      <c r="D73"/>
+    </row>
+    <row r="74" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B74"/>
+      <c r="C74"/>
+      <c r="D74"/>
+    </row>
+    <row r="75" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B75"/>
+      <c r="C75"/>
+      <c r="D75"/>
+    </row>
+    <row r="76" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C76"/>
+      <c r="D76"/>
+    </row>
+    <row r="77" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C77"/>
+      <c r="D77"/>
+    </row>
+    <row r="78" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C78"/>
+      <c r="D78"/>
+    </row>
+    <row r="79" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C79"/>
+      <c r="D79"/>
+    </row>
+    <row r="80" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C80"/>
+      <c r="D80"/>
+    </row>
+    <row r="81" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C81"/>
+      <c r="D81"/>
+    </row>
+    <row r="82" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C82"/>
+      <c r="D82"/>
+    </row>
+    <row r="83" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C83"/>
+      <c r="D83"/>
+    </row>
+    <row r="84" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C84"/>
+      <c r="D84"/>
+    </row>
+    <row r="85" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C85"/>
+      <c r="D85"/>
+    </row>
+    <row r="86" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C86"/>
+      <c r="D86"/>
+    </row>
+    <row r="87" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C87"/>
+      <c r="D87"/>
+    </row>
+    <row r="88" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C88"/>
+      <c r="D88"/>
+    </row>
+    <row r="89" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C89"/>
+      <c r="D89"/>
+    </row>
+    <row r="90" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C90"/>
+      <c r="D90"/>
+    </row>
+    <row r="91" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C91"/>
+      <c r="D91"/>
+    </row>
+    <row r="92" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C92"/>
+      <c r="D92"/>
+    </row>
+    <row r="93" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C93"/>
+      <c r="D93"/>
+    </row>
+    <row r="94" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C94"/>
+      <c r="D94"/>
+    </row>
+    <row r="95" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C95"/>
+      <c r="D95"/>
+    </row>
+    <row r="96" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C96"/>
+      <c r="D96"/>
+    </row>
+    <row r="97" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C97"/>
+      <c r="D97"/>
+    </row>
+    <row r="98" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C98"/>
+      <c r="D98"/>
+    </row>
+    <row r="99" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C99"/>
+      <c r="D99"/>
+    </row>
+    <row r="100" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C100"/>
+      <c r="D100"/>
+    </row>
+    <row r="101" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C101"/>
+      <c r="D101"/>
+    </row>
+    <row r="102" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C102"/>
+      <c r="D102"/>
+    </row>
+    <row r="103" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C103"/>
+      <c r="D103"/>
+    </row>
+    <row r="104" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C104"/>
+      <c r="D104"/>
+    </row>
+    <row r="105" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C105"/>
+      <c r="D105"/>
+    </row>
+    <row r="106" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C106"/>
+      <c r="D106"/>
+    </row>
+    <row r="107" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C107"/>
+      <c r="D107"/>
+    </row>
+    <row r="108" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C108"/>
+      <c r="D108"/>
+    </row>
+    <row r="109" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C109"/>
+      <c r="D109"/>
+    </row>
+    <row r="110" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C110"/>
+      <c r="D110"/>
+    </row>
+    <row r="111" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C111"/>
+      <c r="D111"/>
+    </row>
+    <row r="112" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C112"/>
+      <c r="D112"/>
+    </row>
+    <row r="113" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C113"/>
+      <c r="D113"/>
+    </row>
+    <row r="114" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C114"/>
+      <c r="D114"/>
+    </row>
+    <row r="115" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C115"/>
+      <c r="D115"/>
+    </row>
+    <row r="116" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C116"/>
+      <c r="D116"/>
+    </row>
+    <row r="117" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C117"/>
+      <c r="D117"/>
+    </row>
+    <row r="118" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C118"/>
+      <c r="D118"/>
+    </row>
+    <row r="119" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C119"/>
+      <c r="D119"/>
+    </row>
+    <row r="120" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C120"/>
+      <c r="D120"/>
+    </row>
+    <row r="121" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C121"/>
+      <c r="D121"/>
+    </row>
+    <row r="122" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C122"/>
+      <c r="D122"/>
+    </row>
+    <row r="123" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C123"/>
+      <c r="D123"/>
+    </row>
+    <row r="124" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C124"/>
+      <c r="D124"/>
+    </row>
+    <row r="125" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C125"/>
+      <c r="D125"/>
+    </row>
+    <row r="126" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C126"/>
+      <c r="D126"/>
+    </row>
+    <row r="127" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C127"/>
+      <c r="D127"/>
+    </row>
+    <row r="128" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C128"/>
+      <c r="D128"/>
+    </row>
+    <row r="129" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C129"/>
+      <c r="D129"/>
+    </row>
+    <row r="130" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C130"/>
+      <c r="D130"/>
+    </row>
+    <row r="131" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C131"/>
+      <c r="D131"/>
+    </row>
+    <row r="132" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C132"/>
+      <c r="D132"/>
+    </row>
+    <row r="133" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C133"/>
+      <c r="D133"/>
+    </row>
+    <row r="134" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C134"/>
+      <c r="D134"/>
+    </row>
+    <row r="135" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C135"/>
+      <c r="D135"/>
+    </row>
+    <row r="136" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C136"/>
+      <c r="D136"/>
+    </row>
+    <row r="137" spans="3:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C137"/>
+      <c r="D137"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K35">
+  <autoFilter ref="A1:K34" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K34">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>

</xml_diff>